<commit_message>
Fixed accidental swap of Lesson 4 examples
</commit_message>
<xml_diff>
--- a/doc/Tutorial/Lesson-4/Example-4.1/Items.xlsx
+++ b/doc/Tutorial/Lesson-4/Example-4.1/Items.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t xml:space="preserve">Record Type</t>
   </si>
@@ -68,73 +68,18 @@
     <t xml:space="preserve">Doodad Test</t>
   </si>
   <si>
-    <t xml:space="preserve">T:Test Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Operator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Operator Note</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Overall Status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subtest Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trial Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trial Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Result</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">heavy snow</t>
+    <t xml:space="preserve">DATA</t>
   </si>
   <si>
     <t xml:space="preserve">pass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bounce</t>
-  </si>
-  <si>
-    <t xml:space="preserve">drop from 1 meter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">drop from 2 meter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">smash</t>
-  </si>
-  <si>
-    <t xml:space="preserve">smash with 5# hammer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">smash with 9# hammer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bill</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cold, windy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SN000002</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -235,7 +180,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -254,14 +199,6 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -420,37 +357,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="13.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.09"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -466,7 +390,6 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
@@ -482,23 +405,14 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
@@ -507,238 +421,19 @@
       <c r="B6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="6" t="n">
-        <v>45373.3645833333</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="I7" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="6" t="n">
-        <v>45373.3645833333</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="6" t="n">
-        <v>45373.3645833333</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="G9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="I9" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="6" t="n">
-        <v>45373.3645833333</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="I10" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="6" t="n">
-        <v>45380.5833333333</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="G11" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="I11" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="6" t="n">
-        <v>45380.5833333333</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="H12" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="I12" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="6" t="n">
-        <v>45380.5833333333</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="G13" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="I13" s="0" t="s">
-        <v>25</v>
+      <c r="B7" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="B1:J1"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="B4:J4"/>
-    <mergeCell ref="A5:J5"/>
+  <mergeCells count="2">
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:I3"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>